<commit_message>
RKI-1 changed in DD_BGS98 sheet names and added "variable", "name", "label" to sheet "categories"
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_dictionary/DD_BGS98_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_dictionary/DD_BGS98_FRANZI.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10466767-0A66-4235-BFD9-7161499914E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BF057-A72E-4E3C-9243-3D4503B6ECFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{78138994-0646-4D67-A212-39C531A38F77}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{78138994-0646-4D67-A212-39C531A38F77}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>index</t>
   </si>
@@ -322,6 +323,9 @@
   </si>
   <si>
     <t>Gekochte Kartoffeln</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -712,16 +716,16 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -746,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -757,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -768,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -779,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -790,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -801,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -812,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -823,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -834,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -845,7 +849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -856,7 +860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -867,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -878,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -889,7 +893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -900,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -911,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -922,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -933,7 +937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -944,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>24</v>
       </c>
@@ -955,7 +959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>25</v>
       </c>
@@ -966,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>26</v>
@@ -978,7 +982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>27</v>
@@ -990,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>28</v>
@@ -1002,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
         <v>29</v>
@@ -1014,7 +1018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>30</v>
@@ -1026,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>31</v>
@@ -1038,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
         <v>32</v>
@@ -1050,7 +1054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
         <v>33</v>
@@ -1062,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -1073,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>35</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>37</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>38</v>
       </c>
@@ -1117,7 +1121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>39</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>40</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>41</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -1161,7 +1165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>43</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>44</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>45</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>46</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>47</v>
       </c>
@@ -1227,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>49</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>51</v>
       </c>
@@ -1260,277 +1264,277 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -1539,4 +1543,30 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D01290-A2A0-4F25-A7B5-A3DD9AF84092}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>